<commit_message>
connect model with design CORE
</commit_message>
<xml_diff>
--- a/em_kette_stanag2021.xlsx
+++ b/em_kette_stanag2021.xlsx
@@ -8,17 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\Pythonecke\BB_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE855D0C-F2C2-4F68-AA11-78B676CA45CE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE3F703-FC21-482F-B73B-0F65648CD800}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31440" yWindow="15" windowWidth="18345" windowHeight="13755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -27,46 +33,46 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>mlc4</t>
+    <t>MLC4</t>
   </si>
   <si>
-    <t>mlc8</t>
+    <t>MLC8</t>
   </si>
   <si>
-    <t>mlc12</t>
+    <t>MLC12</t>
   </si>
   <si>
-    <t>mlc16</t>
+    <t>MLC16</t>
   </si>
   <si>
-    <t>mlc20</t>
+    <t>MLC20</t>
   </si>
   <si>
-    <t>mlc24</t>
+    <t>MLC24</t>
   </si>
   <si>
-    <t>mlc30</t>
+    <t>MLC30</t>
   </si>
   <si>
-    <t>mlc40</t>
+    <t>MLC40</t>
   </si>
   <si>
-    <t>mlc50</t>
+    <t>MLC50</t>
   </si>
   <si>
-    <t>mlc60</t>
+    <t>MLC60</t>
   </si>
   <si>
-    <t>mlc70</t>
+    <t>MLC70</t>
   </si>
   <si>
-    <t>mlc80</t>
+    <t>MLC80</t>
   </si>
   <si>
-    <t>mlc90</t>
+    <t>MLC90</t>
   </si>
   <si>
-    <t>mlc100</t>
+    <t>MLC100</t>
   </si>
 </sst>
 </file>
@@ -82,12 +88,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -102,9 +114,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -385,9 +398,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -437,49 +452,49 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>2.4300000000000002</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>4.5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>4.87</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2">
         <v>6.49</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2">
         <v>8.1199999999999992</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2">
         <v>9.74</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2">
         <v>9.9600000000000009</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2">
         <v>12.16</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2">
         <v>14.05</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2">
         <v>15.63</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2">
         <v>17.04</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2">
         <v>18.239999999999998</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2">
         <v>19.329999999999998</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2">
         <v>20.260000000000002</v>
       </c>
     </row>
@@ -955,659 +970,903 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>7.74</v>
-      </c>
-      <c r="C13">
-        <v>15.29</v>
-      </c>
-      <c r="D13">
-        <v>21.46</v>
-      </c>
-      <c r="E13">
-        <v>28.62</v>
-      </c>
-      <c r="F13">
-        <v>35.78</v>
-      </c>
-      <c r="G13">
-        <v>42.94</v>
-      </c>
-      <c r="H13">
-        <v>50.78</v>
-      </c>
-      <c r="I13">
-        <v>65.73</v>
-      </c>
-      <c r="J13">
-        <v>79.78</v>
-      </c>
-      <c r="K13">
-        <v>92.78</v>
-      </c>
-      <c r="L13">
-        <v>104.9</v>
-      </c>
-      <c r="M13">
-        <v>115.96</v>
-      </c>
-      <c r="N13">
-        <v>126.16</v>
-      </c>
-      <c r="O13">
-        <v>135.24</v>
+        <v>6.5</v>
+      </c>
+      <c r="B13" s="2">
+        <f>(B12+(B14-B12)/2)</f>
+        <v>7.6449999999999996</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" ref="C13:O13" si="0">(C12+(C14-C12)/2)</f>
+        <v>15.079999999999998</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>21.024999999999999</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>28.04</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>35.055</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>42.07</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>49.45</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="0"/>
+        <v>63.795000000000002</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="0"/>
+        <v>77.155000000000001</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="0"/>
+        <v>89.384999999999991</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="0"/>
+        <v>100.66500000000001</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="0"/>
+        <v>110.78999999999999</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="0"/>
+        <v>119.985</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="0"/>
+        <v>127.97</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14">
-        <v>7.88</v>
+        <v>7.74</v>
       </c>
       <c r="C14">
-        <v>15.6</v>
+        <v>15.29</v>
       </c>
       <c r="D14">
-        <v>22.11</v>
+        <v>21.46</v>
       </c>
       <c r="E14">
-        <v>29.49</v>
+        <v>28.62</v>
       </c>
       <c r="F14">
-        <v>36.869999999999997</v>
+        <v>35.78</v>
       </c>
       <c r="G14">
-        <v>44.25</v>
+        <v>42.94</v>
       </c>
       <c r="H14">
-        <v>52.78</v>
+        <v>50.78</v>
       </c>
       <c r="I14">
-        <v>68.64</v>
+        <v>65.73</v>
       </c>
       <c r="J14">
-        <v>83.71</v>
+        <v>79.78</v>
       </c>
       <c r="K14">
-        <v>97.87</v>
+        <v>92.78</v>
       </c>
       <c r="L14">
-        <v>111.25</v>
+        <v>104.9</v>
       </c>
       <c r="M14">
-        <v>123.71</v>
+        <v>115.96</v>
       </c>
       <c r="N14">
-        <v>135.41999999999999</v>
+        <v>126.16</v>
       </c>
       <c r="O14">
-        <v>146.15</v>
+        <v>135.24</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>9</v>
-      </c>
-      <c r="B15">
-        <v>8</v>
-      </c>
-      <c r="C15">
-        <v>15.85</v>
-      </c>
-      <c r="D15">
-        <v>22.62</v>
-      </c>
-      <c r="E15">
-        <v>30.17</v>
-      </c>
-      <c r="F15">
-        <v>37.72</v>
-      </c>
-      <c r="G15">
-        <v>45.26</v>
-      </c>
-      <c r="H15">
-        <v>54.33</v>
-      </c>
-      <c r="I15">
-        <v>70.900000000000006</v>
-      </c>
-      <c r="J15">
-        <v>86.77</v>
-      </c>
-      <c r="K15">
-        <v>101.82</v>
-      </c>
-      <c r="L15">
-        <v>116.2</v>
-      </c>
-      <c r="M15">
-        <v>129.74</v>
-      </c>
-      <c r="N15">
-        <v>142.62</v>
-      </c>
-      <c r="O15">
-        <v>154.63</v>
+        <v>7.5</v>
+      </c>
+      <c r="B15" s="2">
+        <f>(B14+(B16-B14)/2)</f>
+        <v>7.8100000000000005</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" ref="C15:O15" si="1">(C14+(C16-C14)/2)</f>
+        <v>15.445</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="1"/>
+        <v>21.785</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>29.055</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="1"/>
+        <v>36.325000000000003</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="1"/>
+        <v>43.594999999999999</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>51.78</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>67.185000000000002</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="1"/>
+        <v>81.745000000000005</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="1"/>
+        <v>95.325000000000003</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="1"/>
+        <v>108.075</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="1"/>
+        <v>119.83499999999999</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="1"/>
+        <v>130.79</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="1"/>
+        <v>140.69499999999999</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16">
-        <v>8.09</v>
+        <v>7.88</v>
       </c>
       <c r="C16">
-        <v>16.04</v>
+        <v>15.6</v>
       </c>
       <c r="D16">
-        <v>23.03</v>
+        <v>22.11</v>
       </c>
       <c r="E16">
-        <v>30.71</v>
+        <v>29.49</v>
       </c>
       <c r="F16">
-        <v>38.39</v>
+        <v>36.869999999999997</v>
       </c>
       <c r="G16">
-        <v>46.08</v>
+        <v>44.25</v>
       </c>
       <c r="H16">
-        <v>55.58</v>
+        <v>52.78</v>
       </c>
       <c r="I16">
-        <v>72.709999999999994</v>
+        <v>68.64</v>
       </c>
       <c r="J16">
-        <v>89.22</v>
+        <v>83.71</v>
       </c>
       <c r="K16">
-        <v>104.99</v>
+        <v>97.87</v>
       </c>
       <c r="L16">
-        <v>120.15</v>
+        <v>111.25</v>
       </c>
       <c r="M16">
-        <v>134.57</v>
+        <v>123.71</v>
       </c>
       <c r="N16">
-        <v>148.38</v>
+        <v>135.41999999999999</v>
       </c>
       <c r="O16">
-        <v>161.41999999999999</v>
+        <v>146.15</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>11</v>
-      </c>
-      <c r="B17">
-        <v>8.16</v>
-      </c>
-      <c r="C17">
-        <v>16.2</v>
-      </c>
-      <c r="D17">
-        <v>23.36</v>
-      </c>
-      <c r="E17">
-        <v>31.15</v>
-      </c>
-      <c r="F17">
-        <v>38.950000000000003</v>
-      </c>
-      <c r="G17">
-        <v>46.74</v>
-      </c>
-      <c r="H17">
-        <v>56.59</v>
-      </c>
-      <c r="I17">
-        <v>74.2</v>
-      </c>
-      <c r="J17">
-        <v>91.22</v>
-      </c>
-      <c r="K17">
-        <v>107.58</v>
-      </c>
-      <c r="L17">
-        <v>123.38</v>
-      </c>
-      <c r="M17">
-        <v>138.52000000000001</v>
-      </c>
-      <c r="N17">
-        <v>153.1</v>
-      </c>
-      <c r="O17">
-        <v>166.97</v>
+        <v>8.5</v>
+      </c>
+      <c r="B17" s="2">
+        <f>(B16+(B18-B16)/2)</f>
+        <v>7.9399999999999995</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" ref="C17:O17" si="2">(C16+(C18-C16)/2)</f>
+        <v>15.725</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="2"/>
+        <v>22.365000000000002</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="2"/>
+        <v>29.83</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="2"/>
+        <v>37.295000000000002</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="2"/>
+        <v>44.754999999999995</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="2"/>
+        <v>53.555</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="2"/>
+        <v>69.77000000000001</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="2"/>
+        <v>85.24</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="2"/>
+        <v>99.844999999999999</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="2"/>
+        <v>113.72499999999999</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="2"/>
+        <v>126.72499999999999</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="2"/>
+        <v>139.01999999999998</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="2"/>
+        <v>150.38999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B18">
-        <v>8.2200000000000006</v>
+        <v>8</v>
       </c>
       <c r="C18">
-        <v>16.34</v>
+        <v>15.85</v>
       </c>
       <c r="D18">
-        <v>23.64</v>
+        <v>22.62</v>
       </c>
       <c r="E18">
-        <v>31.52</v>
+        <v>30.17</v>
       </c>
       <c r="F18">
-        <v>39.409999999999997</v>
+        <v>37.72</v>
       </c>
       <c r="G18">
-        <v>47.3</v>
+        <v>45.26</v>
       </c>
       <c r="H18">
-        <v>57.44</v>
+        <v>54.33</v>
       </c>
       <c r="I18">
-        <v>75.430000000000007</v>
+        <v>70.900000000000006</v>
       </c>
       <c r="J18">
-        <v>92.89</v>
+        <v>86.77</v>
       </c>
       <c r="K18">
-        <v>109.74</v>
+        <v>101.82</v>
       </c>
       <c r="L18">
-        <v>126.08</v>
+        <v>116.2</v>
       </c>
       <c r="M18">
-        <v>141.81</v>
+        <v>129.74</v>
       </c>
       <c r="N18">
-        <v>157.03</v>
+        <v>142.62</v>
       </c>
       <c r="O18">
-        <v>171.6</v>
+        <v>154.63</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>13</v>
-      </c>
-      <c r="B19">
-        <v>8.2799999999999994</v>
-      </c>
-      <c r="C19">
-        <v>16.45</v>
-      </c>
-      <c r="D19">
-        <v>23.87</v>
-      </c>
-      <c r="E19">
-        <v>31.84</v>
-      </c>
-      <c r="F19">
-        <v>39.799999999999997</v>
-      </c>
-      <c r="G19">
-        <v>47.76</v>
-      </c>
-      <c r="H19">
-        <v>58.16</v>
-      </c>
-      <c r="I19">
-        <v>76.47</v>
-      </c>
-      <c r="J19">
-        <v>94.3</v>
-      </c>
-      <c r="K19">
-        <v>111.57</v>
-      </c>
-      <c r="L19">
-        <v>128.36000000000001</v>
-      </c>
-      <c r="M19">
-        <v>144.59</v>
-      </c>
-      <c r="N19">
-        <v>160.35</v>
-      </c>
-      <c r="O19">
-        <v>175.51</v>
+        <v>9.5</v>
+      </c>
+      <c r="B19" s="2">
+        <f>(B18+(B20-B18)/2)</f>
+        <v>8.0449999999999999</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" ref="C19:O19" si="3">(C18+(C20-C18)/2)</f>
+        <v>15.945</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="3"/>
+        <v>22.825000000000003</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="3"/>
+        <v>30.44</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="3"/>
+        <v>38.055</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="3"/>
+        <v>45.67</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="3"/>
+        <v>54.954999999999998</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="3"/>
+        <v>71.805000000000007</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="3"/>
+        <v>87.995000000000005</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" si="3"/>
+        <v>103.405</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="3"/>
+        <v>118.17500000000001</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="3"/>
+        <v>132.155</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" si="3"/>
+        <v>145.5</v>
+      </c>
+      <c r="O19" s="2">
+        <f t="shared" si="3"/>
+        <v>158.02499999999998</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B20">
-        <v>8.32</v>
+        <v>8.09</v>
       </c>
       <c r="C20">
-        <v>16.55</v>
+        <v>16.04</v>
       </c>
       <c r="D20">
-        <v>24.07</v>
+        <v>23.03</v>
       </c>
       <c r="E20">
-        <v>32.1</v>
+        <v>30.71</v>
       </c>
       <c r="F20">
-        <v>40.14</v>
+        <v>38.39</v>
       </c>
       <c r="G20">
-        <v>48.17</v>
+        <v>46.08</v>
       </c>
       <c r="H20">
-        <v>58.77</v>
+        <v>55.58</v>
       </c>
       <c r="I20">
-        <v>77.37</v>
+        <v>72.709999999999994</v>
       </c>
       <c r="J20">
-        <v>95.51</v>
+        <v>89.22</v>
       </c>
       <c r="K20">
-        <v>113.13</v>
+        <v>104.99</v>
       </c>
       <c r="L20">
-        <v>130.32</v>
+        <v>120.15</v>
       </c>
       <c r="M20">
-        <v>146.97999999999999</v>
+        <v>134.57</v>
       </c>
       <c r="N20">
-        <v>163.19999999999999</v>
+        <v>148.38</v>
       </c>
       <c r="O20">
-        <v>178.87</v>
+        <v>161.41999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B21">
-        <v>8.36</v>
+        <v>8.16</v>
       </c>
       <c r="C21">
-        <v>16.63</v>
+        <v>16.2</v>
       </c>
       <c r="D21">
-        <v>24.25</v>
+        <v>23.36</v>
       </c>
       <c r="E21">
-        <v>32.340000000000003</v>
+        <v>31.15</v>
       </c>
       <c r="F21">
-        <v>40.43</v>
+        <v>38.950000000000003</v>
       </c>
       <c r="G21">
-        <v>48.52</v>
+        <v>46.74</v>
       </c>
       <c r="H21">
-        <v>59.3</v>
+        <v>56.59</v>
       </c>
       <c r="I21">
-        <v>78.14</v>
+        <v>74.2</v>
       </c>
       <c r="J21">
-        <v>96.56</v>
+        <v>91.22</v>
       </c>
       <c r="K21">
-        <v>114.49</v>
+        <v>107.58</v>
       </c>
       <c r="L21">
-        <v>132.01</v>
+        <v>123.38</v>
       </c>
       <c r="M21">
-        <v>149.05000000000001</v>
+        <v>138.52000000000001</v>
       </c>
       <c r="N21">
-        <v>165.67</v>
+        <v>153.1</v>
       </c>
       <c r="O21">
-        <v>181.78</v>
+        <v>166.97</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B22">
-        <v>8.39</v>
+        <v>8.2200000000000006</v>
       </c>
       <c r="C22">
-        <v>16.7</v>
+        <v>16.34</v>
       </c>
       <c r="D22">
-        <v>24.4</v>
+        <v>23.64</v>
       </c>
       <c r="E22">
-        <v>32.54</v>
+        <v>31.52</v>
       </c>
       <c r="F22">
-        <v>40.68</v>
+        <v>39.409999999999997</v>
       </c>
       <c r="G22">
-        <v>48.82</v>
+        <v>47.3</v>
       </c>
       <c r="H22">
-        <v>59.77</v>
+        <v>57.44</v>
       </c>
       <c r="I22">
-        <v>78.819999999999993</v>
+        <v>75.430000000000007</v>
       </c>
       <c r="J22">
-        <v>97.48</v>
+        <v>92.89</v>
       </c>
       <c r="K22">
-        <v>115.68</v>
+        <v>109.74</v>
       </c>
       <c r="L22">
-        <v>133.49</v>
+        <v>126.08</v>
       </c>
       <c r="M22">
-        <v>150.86000000000001</v>
+        <v>141.81</v>
       </c>
       <c r="N22">
-        <v>167.83</v>
+        <v>157.03</v>
       </c>
       <c r="O22">
-        <v>184.32</v>
+        <v>171.6</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B23">
-        <v>8.42</v>
+        <v>8.2799999999999994</v>
       </c>
       <c r="C23">
-        <v>16.77</v>
+        <v>16.45</v>
       </c>
       <c r="D23">
-        <v>24.53</v>
+        <v>23.87</v>
       </c>
       <c r="E23">
-        <v>32.72</v>
+        <v>31.84</v>
       </c>
       <c r="F23">
-        <v>40.9</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="G23">
-        <v>49.09</v>
+        <v>47.76</v>
       </c>
       <c r="H23">
-        <v>60.18</v>
+        <v>58.16</v>
       </c>
       <c r="I23">
-        <v>79.42</v>
+        <v>76.47</v>
       </c>
       <c r="J23">
-        <v>98.29</v>
+        <v>94.3</v>
       </c>
       <c r="K23">
-        <v>116.73</v>
+        <v>111.57</v>
       </c>
       <c r="L23">
-        <v>134.80000000000001</v>
+        <v>128.36000000000001</v>
       </c>
       <c r="M23">
-        <v>152.44999999999999</v>
+        <v>144.59</v>
       </c>
       <c r="N23">
-        <v>169.74</v>
+        <v>160.35</v>
       </c>
       <c r="O23">
-        <v>186.57</v>
+        <v>175.51</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B24">
-        <v>8.4499999999999993</v>
+        <v>8.32</v>
       </c>
       <c r="C24">
-        <v>16.829999999999998</v>
+        <v>16.55</v>
       </c>
       <c r="D24">
-        <v>24.65</v>
+        <v>24.07</v>
       </c>
       <c r="E24">
-        <v>32.880000000000003</v>
+        <v>32.1</v>
       </c>
       <c r="F24">
-        <v>41.1</v>
+        <v>40.14</v>
       </c>
       <c r="G24">
-        <v>49.33</v>
+        <v>48.17</v>
       </c>
       <c r="H24">
-        <v>60.55</v>
+        <v>58.77</v>
       </c>
       <c r="I24">
-        <v>79.95</v>
+        <v>77.37</v>
       </c>
       <c r="J24">
-        <v>99.01</v>
+        <v>95.51</v>
       </c>
       <c r="K24">
-        <v>117.66</v>
+        <v>113.13</v>
       </c>
       <c r="L24">
-        <v>135.96</v>
+        <v>130.32</v>
       </c>
       <c r="M24">
-        <v>153.87</v>
+        <v>146.97999999999999</v>
       </c>
       <c r="N24">
-        <v>171.43</v>
+        <v>163.19999999999999</v>
       </c>
       <c r="O24">
-        <v>188.56</v>
+        <v>178.87</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B25">
-        <v>8.4700000000000006</v>
+        <v>8.36</v>
       </c>
       <c r="C25">
-        <v>16.88</v>
+        <v>16.63</v>
       </c>
       <c r="D25">
-        <v>24.76</v>
+        <v>24.25</v>
       </c>
       <c r="E25">
-        <v>33.020000000000003</v>
+        <v>32.340000000000003</v>
       </c>
       <c r="F25">
-        <v>41.28</v>
+        <v>40.43</v>
       </c>
       <c r="G25">
-        <v>49.54</v>
+        <v>48.52</v>
       </c>
       <c r="H25">
-        <v>60.87</v>
+        <v>59.3</v>
       </c>
       <c r="I25">
-        <v>80.430000000000007</v>
+        <v>78.14</v>
       </c>
       <c r="J25">
-        <v>99.65</v>
+        <v>96.56</v>
       </c>
       <c r="K25">
-        <v>118.49</v>
+        <v>114.49</v>
       </c>
       <c r="L25">
-        <v>137.01</v>
+        <v>132.01</v>
       </c>
       <c r="M25">
-        <v>155.13999999999999</v>
+        <v>149.05000000000001</v>
       </c>
       <c r="N25">
-        <v>172.95</v>
+        <v>165.67</v>
       </c>
       <c r="O25">
-        <v>190.35</v>
+        <v>181.78</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
+        <v>16</v>
+      </c>
+      <c r="B26">
+        <v>8.39</v>
+      </c>
+      <c r="C26">
+        <v>16.7</v>
+      </c>
+      <c r="D26">
+        <v>24.4</v>
+      </c>
+      <c r="E26">
+        <v>32.54</v>
+      </c>
+      <c r="F26">
+        <v>40.68</v>
+      </c>
+      <c r="G26">
+        <v>48.82</v>
+      </c>
+      <c r="H26">
+        <v>59.77</v>
+      </c>
+      <c r="I26">
+        <v>78.819999999999993</v>
+      </c>
+      <c r="J26">
+        <v>97.48</v>
+      </c>
+      <c r="K26">
+        <v>115.68</v>
+      </c>
+      <c r="L26">
+        <v>133.49</v>
+      </c>
+      <c r="M26">
+        <v>150.86000000000001</v>
+      </c>
+      <c r="N26">
+        <v>167.83</v>
+      </c>
+      <c r="O26">
+        <v>184.32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>17</v>
+      </c>
+      <c r="B27">
+        <v>8.42</v>
+      </c>
+      <c r="C27">
+        <v>16.77</v>
+      </c>
+      <c r="D27">
+        <v>24.53</v>
+      </c>
+      <c r="E27">
+        <v>32.72</v>
+      </c>
+      <c r="F27">
+        <v>40.9</v>
+      </c>
+      <c r="G27">
+        <v>49.09</v>
+      </c>
+      <c r="H27">
+        <v>60.18</v>
+      </c>
+      <c r="I27">
+        <v>79.42</v>
+      </c>
+      <c r="J27">
+        <v>98.29</v>
+      </c>
+      <c r="K27">
+        <v>116.73</v>
+      </c>
+      <c r="L27">
+        <v>134.80000000000001</v>
+      </c>
+      <c r="M27">
+        <v>152.44999999999999</v>
+      </c>
+      <c r="N27">
+        <v>169.74</v>
+      </c>
+      <c r="O27">
+        <v>186.57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>18</v>
+      </c>
+      <c r="B28">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="C28">
+        <v>16.829999999999998</v>
+      </c>
+      <c r="D28">
+        <v>24.65</v>
+      </c>
+      <c r="E28">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="F28">
+        <v>41.1</v>
+      </c>
+      <c r="G28">
+        <v>49.33</v>
+      </c>
+      <c r="H28">
+        <v>60.55</v>
+      </c>
+      <c r="I28">
+        <v>79.95</v>
+      </c>
+      <c r="J28">
+        <v>99.01</v>
+      </c>
+      <c r="K28">
+        <v>117.66</v>
+      </c>
+      <c r="L28">
+        <v>135.96</v>
+      </c>
+      <c r="M28">
+        <v>153.87</v>
+      </c>
+      <c r="N28">
+        <v>171.43</v>
+      </c>
+      <c r="O28">
+        <v>188.56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>19</v>
+      </c>
+      <c r="B29">
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="C29">
+        <v>16.88</v>
+      </c>
+      <c r="D29">
+        <v>24.76</v>
+      </c>
+      <c r="E29">
+        <v>33.020000000000003</v>
+      </c>
+      <c r="F29">
+        <v>41.28</v>
+      </c>
+      <c r="G29">
+        <v>49.54</v>
+      </c>
+      <c r="H29">
+        <v>60.87</v>
+      </c>
+      <c r="I29">
+        <v>80.430000000000007</v>
+      </c>
+      <c r="J29">
+        <v>99.65</v>
+      </c>
+      <c r="K29">
+        <v>118.49</v>
+      </c>
+      <c r="L29">
+        <v>137.01</v>
+      </c>
+      <c r="M29">
+        <v>155.13999999999999</v>
+      </c>
+      <c r="N29">
+        <v>172.95</v>
+      </c>
+      <c r="O29">
+        <v>190.35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>20</v>
       </c>
-      <c r="B26">
+      <c r="B30">
         <v>8.5</v>
       </c>
-      <c r="C26">
+      <c r="C30">
         <v>16.920000000000002</v>
       </c>
-      <c r="D26">
+      <c r="D30">
         <v>24.86</v>
       </c>
-      <c r="E26">
+      <c r="E30">
         <v>33.15</v>
       </c>
-      <c r="F26">
+      <c r="F30">
         <v>41.44</v>
       </c>
-      <c r="G26">
+      <c r="G30">
         <v>49.73</v>
       </c>
-      <c r="H26">
+      <c r="H30">
         <v>61.17</v>
       </c>
-      <c r="I26">
+      <c r="I30">
         <v>80.86</v>
       </c>
-      <c r="J26">
+      <c r="J30">
         <v>100.23</v>
       </c>
-      <c r="K26">
+      <c r="K30">
         <v>119.24</v>
       </c>
-      <c r="L26">
+      <c r="L30">
         <v>137.94</v>
       </c>
-      <c r="M26">
+      <c r="M30">
         <v>156.29</v>
       </c>
-      <c r="N26">
+      <c r="N30">
         <v>174.32</v>
       </c>
-      <c r="O26">
+      <c r="O30">
         <v>191.95</v>
       </c>
     </row>

</xml_diff>